<commit_message>
SI study 6 added
</commit_message>
<xml_diff>
--- a/HypocrisyStudySI_5.xlsx
+++ b/HypocrisyStudySI_5.xlsx
@@ -1,26 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elizabethhuppert/Desktop/preferences-for-moral-absolutism/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C0B0AB03-9CFA-6743-AE35-8C1C9E27EE1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0728339-43C0-D842-983F-4276E0BBEFE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16640"/>
+    <workbookView xWindow="760" yWindow="540" windowWidth="28040" windowHeight="16600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HypocrisyStudySI_5" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HypocrisyStudySI_5!$AO$1:$AO$197</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5315" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5318" uniqueCount="270">
   <si>
     <t>id</t>
   </si>
@@ -825,12 +839,21 @@
   </si>
   <si>
     <t>jhjhk</t>
+  </si>
+  <si>
+    <t>Advice_num</t>
+  </si>
+  <si>
+    <t>Advice_denom</t>
+  </si>
+  <si>
+    <t>advice</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1667,16 +1690,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL197"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AO197"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AO198" sqref="AO198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="30" width="10.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1791,8 +1817,17 @@
       <c r="AL1" t="s">
         <v>37</v>
       </c>
+      <c r="AM1" t="s">
+        <v>267</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>268</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>269</v>
+      </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1907,8 +1942,20 @@
       <c r="AL2">
         <v>2</v>
       </c>
+      <c r="AM2">
+        <f>ABS(SUM(AE2-C2))</f>
+        <v>5</v>
+      </c>
+      <c r="AN2">
+        <f>ABS(SUM(9.24 - C2))</f>
+        <v>5.74</v>
+      </c>
+      <c r="AO2">
+        <f>SUM(AM2/AN2)</f>
+        <v>0.87108013937282225</v>
+      </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2014,8 +2061,20 @@
       <c r="AL3">
         <v>2</v>
       </c>
+      <c r="AM3">
+        <f t="shared" ref="AM3:AM66" si="0">ABS(SUM(AE3-C3))</f>
+        <v>0</v>
+      </c>
+      <c r="AN3">
+        <f>ABS(SUM(9.24 - C3))</f>
+        <v>10.76</v>
+      </c>
+      <c r="AO3">
+        <f t="shared" ref="AO3:AO66" si="1">SUM(AM3/AN3)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2121,8 +2180,20 @@
       <c r="AL4">
         <v>2</v>
       </c>
+      <c r="AM4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AN4">
+        <f>ABS(SUM(9.24 - C4))</f>
+        <v>8.24</v>
+      </c>
+      <c r="AO4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2228,8 +2299,20 @@
       <c r="AL5">
         <v>2</v>
       </c>
+      <c r="AM5">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="AN5">
+        <f>ABS(SUM(9.24 - C5))</f>
+        <v>4.74</v>
+      </c>
+      <c r="AO5">
+        <f t="shared" si="1"/>
+        <v>0.31645569620253161</v>
+      </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2344,8 +2427,20 @@
       <c r="AL6">
         <v>2</v>
       </c>
+      <c r="AM6">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999978</v>
+      </c>
+      <c r="AN6">
+        <f>ABS(SUM(9.24 - C6))</f>
+        <v>7.38</v>
+      </c>
+      <c r="AO6">
+        <f t="shared" si="1"/>
+        <v>0.1355013550135501</v>
+      </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2460,8 +2555,20 @@
       <c r="AL7">
         <v>2</v>
       </c>
+      <c r="AM7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AN7">
+        <f t="shared" ref="AN7:AN70" si="2">ABS(SUM(9.24 - C7))</f>
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="AO7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2567,8 +2674,20 @@
       <c r="AL8">
         <v>2</v>
       </c>
+      <c r="AM8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AN8">
+        <f t="shared" si="2"/>
+        <v>5.24</v>
+      </c>
+      <c r="AO8">
+        <f t="shared" si="1"/>
+        <v>0.38167938931297707</v>
+      </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2674,8 +2793,20 @@
       <c r="AL9">
         <v>2</v>
       </c>
+      <c r="AM9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AN9">
+        <f t="shared" si="2"/>
+        <v>6.24</v>
+      </c>
+      <c r="AO9">
+        <f t="shared" si="1"/>
+        <v>0.16025641025641024</v>
+      </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2781,8 +2912,20 @@
       <c r="AL10">
         <v>2</v>
       </c>
+      <c r="AM10">
+        <f t="shared" si="0"/>
+        <v>4.24</v>
+      </c>
+      <c r="AN10">
+        <f t="shared" si="2"/>
+        <v>4.24</v>
+      </c>
+      <c r="AO10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:41" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2897,8 +3040,20 @@
       <c r="AL11">
         <v>2</v>
       </c>
+      <c r="AM11">
+        <f t="shared" si="0"/>
+        <v>1.7300000000000004</v>
+      </c>
+      <c r="AN11">
+        <f t="shared" si="2"/>
+        <v>1.7300000000000004</v>
+      </c>
+      <c r="AO11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3004,8 +3159,20 @@
       <c r="AL12">
         <v>2</v>
       </c>
+      <c r="AM12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AN12">
+        <f t="shared" si="2"/>
+        <v>5.76</v>
+      </c>
+      <c r="AO12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3111,8 +3278,20 @@
       <c r="AL13">
         <v>2</v>
       </c>
+      <c r="AM13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AN13">
+        <f t="shared" si="2"/>
+        <v>6.24</v>
+      </c>
+      <c r="AO13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3218,8 +3397,20 @@
       <c r="AL14">
         <v>2</v>
       </c>
+      <c r="AM14">
+        <f t="shared" si="0"/>
+        <v>7.24</v>
+      </c>
+      <c r="AN14">
+        <f t="shared" si="2"/>
+        <v>7.24</v>
+      </c>
+      <c r="AO14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3334,8 +3525,20 @@
       <c r="AL15">
         <v>2</v>
       </c>
+      <c r="AM15">
+        <f t="shared" si="0"/>
+        <v>4.24</v>
+      </c>
+      <c r="AN15">
+        <f t="shared" si="2"/>
+        <v>4.24</v>
+      </c>
+      <c r="AO15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3441,8 +3644,20 @@
       <c r="AL16">
         <v>2</v>
       </c>
+      <c r="AM16">
+        <f t="shared" si="0"/>
+        <v>1.17</v>
+      </c>
+      <c r="AN16">
+        <f t="shared" si="2"/>
+        <v>3.74</v>
+      </c>
+      <c r="AO16">
+        <f t="shared" si="1"/>
+        <v>0.31283422459893045</v>
+      </c>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3557,8 +3772,20 @@
       <c r="AL17">
         <v>2</v>
       </c>
+      <c r="AM17">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="AN17">
+        <f t="shared" si="2"/>
+        <v>4.24</v>
+      </c>
+      <c r="AO17">
+        <f t="shared" si="1"/>
+        <v>0.94339622641509424</v>
+      </c>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3664,8 +3891,20 @@
       <c r="AL18">
         <v>2</v>
       </c>
+      <c r="AM18">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="AN18">
+        <f t="shared" si="2"/>
+        <v>7.74</v>
+      </c>
+      <c r="AO18">
+        <f t="shared" si="1"/>
+        <v>0.45219638242894056</v>
+      </c>
     </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3771,8 +4010,20 @@
       <c r="AL19">
         <v>2</v>
       </c>
+      <c r="AM19">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="AN19">
+        <f t="shared" si="2"/>
+        <v>4.24</v>
+      </c>
+      <c r="AO19">
+        <f t="shared" si="1"/>
+        <v>0.82547169811320753</v>
+      </c>
     </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3887,8 +4138,20 @@
       <c r="AL20">
         <v>2</v>
       </c>
+      <c r="AM20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AN20">
+        <f t="shared" si="2"/>
+        <v>7.24</v>
+      </c>
+      <c r="AO20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3994,8 +4257,20 @@
       <c r="AL21">
         <v>2</v>
       </c>
+      <c r="AM21">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="AN21">
+        <f t="shared" si="2"/>
+        <v>50.76</v>
+      </c>
+      <c r="AO21">
+        <f t="shared" si="1"/>
+        <v>1.0047281323877069</v>
+      </c>
     </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4101,8 +4376,20 @@
       <c r="AL22">
         <v>2</v>
       </c>
+      <c r="AM22">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="AN22">
+        <f t="shared" si="2"/>
+        <v>7.24</v>
+      </c>
+      <c r="AO22">
+        <f t="shared" si="1"/>
+        <v>6.9060773480662987E-2</v>
+      </c>
     </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4208,8 +4495,20 @@
       <c r="AL23">
         <v>2</v>
       </c>
+      <c r="AM23">
+        <f t="shared" si="0"/>
+        <v>2.25</v>
+      </c>
+      <c r="AN23">
+        <f t="shared" si="2"/>
+        <v>6.99</v>
+      </c>
+      <c r="AO23">
+        <f t="shared" si="1"/>
+        <v>0.32188841201716739</v>
+      </c>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4315,8 +4614,20 @@
       <c r="AL24">
         <v>2</v>
       </c>
+      <c r="AM24">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AN24">
+        <f t="shared" si="2"/>
+        <v>4.24</v>
+      </c>
+      <c r="AO24">
+        <f t="shared" si="1"/>
+        <v>0.47169811320754712</v>
+      </c>
     </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -4422,8 +4733,20 @@
       <c r="AL25">
         <v>2</v>
       </c>
+      <c r="AM25">
+        <f t="shared" si="0"/>
+        <v>6.75</v>
+      </c>
+      <c r="AN25">
+        <f t="shared" si="2"/>
+        <v>7.74</v>
+      </c>
+      <c r="AO25">
+        <f t="shared" si="1"/>
+        <v>0.87209302325581395</v>
+      </c>
     </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -4529,8 +4852,20 @@
       <c r="AL26">
         <v>2</v>
       </c>
+      <c r="AM26">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AN26">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="AO26">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4636,8 +4971,20 @@
       <c r="AL27">
         <v>1</v>
       </c>
+      <c r="AM27">
+        <f t="shared" si="0"/>
+        <v>109</v>
+      </c>
+      <c r="AN27">
+        <f t="shared" si="2"/>
+        <v>110.76</v>
+      </c>
+      <c r="AO27">
+        <f t="shared" si="1"/>
+        <v>0.98410978692668827</v>
+      </c>
     </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4743,8 +5090,20 @@
       <c r="AL28">
         <v>1</v>
       </c>
+      <c r="AM28">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="AN28">
+        <f t="shared" si="2"/>
+        <v>20.759999999999998</v>
+      </c>
+      <c r="AO28">
+        <f t="shared" si="1"/>
+        <v>0.96339113680154154</v>
+      </c>
     </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4850,8 +5209,20 @@
       <c r="AL29">
         <v>2</v>
       </c>
+      <c r="AM29">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AN29">
+        <f t="shared" si="2"/>
+        <v>4.99</v>
+      </c>
+      <c r="AO29">
+        <f t="shared" si="1"/>
+        <v>0.40080160320641278</v>
+      </c>
     </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4966,8 +5337,20 @@
       <c r="AL30">
         <v>2</v>
       </c>
+      <c r="AM30">
+        <f t="shared" si="0"/>
+        <v>2.3899999999999997</v>
+      </c>
+      <c r="AN30">
+        <f t="shared" si="2"/>
+        <v>4.71</v>
+      </c>
+      <c r="AO30">
+        <f t="shared" si="1"/>
+        <v>0.50743099787685764</v>
+      </c>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -5082,8 +5465,20 @@
       <c r="AL31">
         <v>2</v>
       </c>
+      <c r="AM31">
+        <f t="shared" si="0"/>
+        <v>0.74000000000000021</v>
+      </c>
+      <c r="AN31">
+        <f t="shared" si="2"/>
+        <v>0.74000000000000021</v>
+      </c>
+      <c r="AO31">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -5189,8 +5584,20 @@
       <c r="AL32">
         <v>2</v>
       </c>
+      <c r="AM32">
+        <f t="shared" si="0"/>
+        <v>0.40000000000000036</v>
+      </c>
+      <c r="AN32">
+        <f t="shared" si="2"/>
+        <v>3.4400000000000004</v>
+      </c>
+      <c r="AO32">
+        <f t="shared" si="1"/>
+        <v>0.11627906976744196</v>
+      </c>
     </row>
-    <row r="33" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -5305,8 +5712,20 @@
       <c r="AL33">
         <v>2</v>
       </c>
+      <c r="AM33">
+        <f t="shared" si="0"/>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="AN33">
+        <f t="shared" si="2"/>
+        <v>5.49</v>
+      </c>
+      <c r="AO33">
+        <f t="shared" si="1"/>
+        <v>0.21857923497267762</v>
+      </c>
     </row>
-    <row r="34" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -5412,8 +5831,20 @@
       <c r="AL34">
         <v>1</v>
       </c>
+      <c r="AM34">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="AN34">
+        <f t="shared" si="2"/>
+        <v>45.76</v>
+      </c>
+      <c r="AO34">
+        <f t="shared" si="1"/>
+        <v>0.98339160839160844</v>
+      </c>
     </row>
-    <row r="35" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -5519,8 +5950,20 @@
       <c r="AL35">
         <v>1</v>
       </c>
+      <c r="AM35">
+        <f t="shared" si="0"/>
+        <v>440.76</v>
+      </c>
+      <c r="AN35">
+        <f t="shared" si="2"/>
+        <v>440.76</v>
+      </c>
+      <c r="AO35">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="36" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -5635,8 +6078,20 @@
       <c r="AL36">
         <v>2</v>
       </c>
+      <c r="AM36">
+        <f t="shared" si="0"/>
+        <v>6.74</v>
+      </c>
+      <c r="AN36">
+        <f t="shared" si="2"/>
+        <v>6.74</v>
+      </c>
+      <c r="AO36">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="37" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -5742,8 +6197,20 @@
       <c r="AL37">
         <v>2</v>
       </c>
+      <c r="AM37">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="AN37">
+        <f t="shared" si="2"/>
+        <v>12.76</v>
+      </c>
+      <c r="AO37">
+        <f t="shared" si="1"/>
+        <v>0.94043887147335425</v>
+      </c>
     </row>
-    <row r="38" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -5858,8 +6325,20 @@
       <c r="AL38">
         <v>2</v>
       </c>
+      <c r="AM38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AN38">
+        <f t="shared" si="2"/>
+        <v>7.24</v>
+      </c>
+      <c r="AO38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="39" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -5965,8 +6444,20 @@
       <c r="AL39">
         <v>1</v>
       </c>
+      <c r="AM39">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="AN39">
+        <f t="shared" si="2"/>
+        <v>50.76</v>
+      </c>
+      <c r="AO39">
+        <f t="shared" si="1"/>
+        <v>0.59101654846335705</v>
+      </c>
     </row>
-    <row r="40" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -6072,8 +6563,20 @@
       <c r="AL40">
         <v>2</v>
       </c>
+      <c r="AM40">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="AN40">
+        <f t="shared" si="2"/>
+        <v>2.74</v>
+      </c>
+      <c r="AO40">
+        <f t="shared" si="1"/>
+        <v>0.91240875912408748</v>
+      </c>
     </row>
-    <row r="41" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -6179,8 +6682,20 @@
       <c r="AL41">
         <v>2</v>
       </c>
+      <c r="AM41">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AN41">
+        <f t="shared" si="2"/>
+        <v>7.24</v>
+      </c>
+      <c r="AO41">
+        <f t="shared" si="1"/>
+        <v>0.13812154696132597</v>
+      </c>
     </row>
-    <row r="42" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -6286,8 +6801,20 @@
       <c r="AL42">
         <v>1</v>
       </c>
+      <c r="AM42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AN42">
+        <f t="shared" si="2"/>
+        <v>190.76</v>
+      </c>
+      <c r="AO42">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="43" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -6393,8 +6920,20 @@
       <c r="AL43">
         <v>2</v>
       </c>
+      <c r="AM43">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AN43">
+        <f t="shared" si="2"/>
+        <v>6.24</v>
+      </c>
+      <c r="AO43">
+        <f t="shared" si="1"/>
+        <v>0.32051282051282048</v>
+      </c>
     </row>
-    <row r="44" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -6500,8 +7039,20 @@
       <c r="AL44">
         <v>2</v>
       </c>
+      <c r="AM44">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AN44">
+        <f t="shared" si="2"/>
+        <v>4.24</v>
+      </c>
+      <c r="AO44">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="45" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -6616,8 +7167,20 @@
       <c r="AL45">
         <v>1</v>
       </c>
+      <c r="AM45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AN45">
+        <f t="shared" si="2"/>
+        <v>10.76</v>
+      </c>
+      <c r="AO45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="46" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -6732,8 +7295,20 @@
       <c r="AL46">
         <v>1</v>
       </c>
+      <c r="AM46">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="AN46">
+        <f t="shared" si="2"/>
+        <v>90.76</v>
+      </c>
+      <c r="AO46">
+        <f t="shared" si="1"/>
+        <v>0.99162626707800783</v>
+      </c>
     </row>
-    <row r="47" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -6839,8 +7414,20 @@
       <c r="AL47">
         <v>2</v>
       </c>
+      <c r="AM47">
+        <f t="shared" si="0"/>
+        <v>7.24</v>
+      </c>
+      <c r="AN47">
+        <f t="shared" si="2"/>
+        <v>7.24</v>
+      </c>
+      <c r="AO47">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="48" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -6955,8 +7542,20 @@
       <c r="AL48">
         <v>1</v>
       </c>
+      <c r="AM48">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="AN48">
+        <f t="shared" si="2"/>
+        <v>240.76</v>
+      </c>
+      <c r="AO48">
+        <f t="shared" si="1"/>
+        <v>0.20767569363681676</v>
+      </c>
     </row>
-    <row r="49" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -7062,8 +7661,20 @@
       <c r="AL49">
         <v>2</v>
       </c>
+      <c r="AM49">
+        <f t="shared" si="0"/>
+        <v>1.0499999999999998</v>
+      </c>
+      <c r="AN49">
+        <f t="shared" si="2"/>
+        <v>5.29</v>
+      </c>
+      <c r="AO49">
+        <f t="shared" si="1"/>
+        <v>0.19848771266540638</v>
+      </c>
     </row>
-    <row r="50" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -7169,8 +7780,20 @@
       <c r="AL50">
         <v>2</v>
       </c>
+      <c r="AM50">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+      <c r="AN50">
+        <f t="shared" si="2"/>
+        <v>6.99</v>
+      </c>
+      <c r="AO50">
+        <f t="shared" si="1"/>
+        <v>0.1072961373390558</v>
+      </c>
     </row>
-    <row r="51" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -7285,8 +7908,20 @@
       <c r="AL51">
         <v>1</v>
       </c>
+      <c r="AM51">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="AN51">
+        <f t="shared" si="2"/>
+        <v>90.76</v>
+      </c>
+      <c r="AO51">
+        <f t="shared" si="1"/>
+        <v>1.1018069634200087</v>
+      </c>
     </row>
-    <row r="52" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -7392,8 +8027,20 @@
       <c r="AL52">
         <v>1</v>
       </c>
+      <c r="AM52">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="AN52">
+        <f t="shared" si="2"/>
+        <v>40.76</v>
+      </c>
+      <c r="AO52">
+        <f t="shared" si="1"/>
+        <v>0.98135426889106969</v>
+      </c>
     </row>
-    <row r="53" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -7499,8 +8146,20 @@
       <c r="AL53">
         <v>2</v>
       </c>
+      <c r="AM53">
+        <f t="shared" si="0"/>
+        <v>4.24</v>
+      </c>
+      <c r="AN53">
+        <f t="shared" si="2"/>
+        <v>4.24</v>
+      </c>
+      <c r="AO53">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="54" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -7606,8 +8265,20 @@
       <c r="AL54">
         <v>1</v>
       </c>
+      <c r="AM54">
+        <f t="shared" si="0"/>
+        <v>1088</v>
+      </c>
+      <c r="AN54">
+        <f t="shared" si="2"/>
+        <v>1090.76</v>
+      </c>
+      <c r="AO54">
+        <f t="shared" si="1"/>
+        <v>0.99746965418607214</v>
+      </c>
     </row>
-    <row r="55" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -7713,8 +8384,20 @@
       <c r="AL55">
         <v>2</v>
       </c>
+      <c r="AM55">
+        <f t="shared" si="0"/>
+        <v>2.7</v>
+      </c>
+      <c r="AN55">
+        <f t="shared" si="2"/>
+        <v>2.7</v>
+      </c>
+      <c r="AO55">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="56" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -7829,8 +8512,20 @@
       <c r="AL56">
         <v>1</v>
       </c>
+      <c r="AM56">
+        <f t="shared" si="0"/>
+        <v>340</v>
+      </c>
+      <c r="AN56">
+        <f t="shared" si="2"/>
+        <v>340.76</v>
+      </c>
+      <c r="AO56">
+        <f t="shared" si="1"/>
+        <v>0.99776969127831905</v>
+      </c>
     </row>
-    <row r="57" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -7936,8 +8631,20 @@
       <c r="AL57">
         <v>1</v>
       </c>
+      <c r="AM57">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="AN57">
+        <f t="shared" si="2"/>
+        <v>1190.76</v>
+      </c>
+      <c r="AO57">
+        <f t="shared" si="1"/>
+        <v>0.16795995834593033</v>
+      </c>
     </row>
-    <row r="58" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -8043,8 +8750,20 @@
       <c r="AL58">
         <v>1</v>
       </c>
+      <c r="AM58">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="AN58">
+        <f t="shared" si="2"/>
+        <v>50.76</v>
+      </c>
+      <c r="AO58">
+        <f t="shared" si="1"/>
+        <v>0.78802206461780933</v>
+      </c>
     </row>
-    <row r="59" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -8150,8 +8869,20 @@
       <c r="AL59">
         <v>2</v>
       </c>
+      <c r="AM59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AN59">
+        <f t="shared" si="2"/>
+        <v>5.03</v>
+      </c>
+      <c r="AO59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="60" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -8257,8 +8988,20 @@
       <c r="AL60">
         <v>1</v>
       </c>
+      <c r="AM60">
+        <f t="shared" si="0"/>
+        <v>875</v>
+      </c>
+      <c r="AN60">
+        <f t="shared" si="2"/>
+        <v>890.76</v>
+      </c>
+      <c r="AO60">
+        <f t="shared" si="1"/>
+        <v>0.9823072432529526</v>
+      </c>
     </row>
-    <row r="61" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -8373,8 +9116,20 @@
       <c r="AL61">
         <v>2</v>
       </c>
+      <c r="AM61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AN61">
+        <f t="shared" si="2"/>
+        <v>4.24</v>
+      </c>
+      <c r="AO61">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="62" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -8489,8 +9244,20 @@
       <c r="AL62">
         <v>2</v>
       </c>
+      <c r="AM62">
+        <f t="shared" si="0"/>
+        <v>4.25</v>
+      </c>
+      <c r="AN62">
+        <f t="shared" si="2"/>
+        <v>5.99</v>
+      </c>
+      <c r="AO62">
+        <f t="shared" si="1"/>
+        <v>0.70951585976627707</v>
+      </c>
     </row>
-    <row r="63" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -8605,8 +9372,20 @@
       <c r="AL63">
         <v>1</v>
       </c>
+      <c r="AM63">
+        <f t="shared" si="0"/>
+        <v>90.7</v>
+      </c>
+      <c r="AN63">
+        <f t="shared" si="2"/>
+        <v>90.76</v>
+      </c>
+      <c r="AO63">
+        <f t="shared" si="1"/>
+        <v>0.999338915821948</v>
+      </c>
     </row>
-    <row r="64" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -8712,8 +9491,20 @@
       <c r="AL64">
         <v>1</v>
       </c>
+      <c r="AM64">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="AN64">
+        <f t="shared" si="2"/>
+        <v>65.760000000000005</v>
+      </c>
+      <c r="AO64">
+        <f t="shared" si="1"/>
+        <v>0.38017031630170312</v>
+      </c>
     </row>
-    <row r="65" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -8819,8 +9610,20 @@
       <c r="AL65">
         <v>2</v>
       </c>
+      <c r="AM65">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AN65">
+        <f t="shared" si="2"/>
+        <v>0.24000000000000021</v>
+      </c>
+      <c r="AO65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="66" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -8935,8 +9738,20 @@
       <c r="AL66">
         <v>2</v>
       </c>
+      <c r="AM66">
+        <f t="shared" si="0"/>
+        <v>4.24</v>
+      </c>
+      <c r="AN66">
+        <f t="shared" si="2"/>
+        <v>4.24</v>
+      </c>
+      <c r="AO66">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="67" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -9051,8 +9866,20 @@
       <c r="AL67">
         <v>2</v>
       </c>
+      <c r="AM67">
+        <f t="shared" ref="AM67:AM130" si="3">ABS(SUM(AE67-C67))</f>
+        <v>3.75</v>
+      </c>
+      <c r="AN67">
+        <f t="shared" si="2"/>
+        <v>4.24</v>
+      </c>
+      <c r="AO67">
+        <f t="shared" ref="AO67:AO130" si="4">SUM(AM67/AN67)</f>
+        <v>0.88443396226415094</v>
+      </c>
     </row>
-    <row r="68" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -9158,8 +9985,20 @@
       <c r="AL68">
         <v>2</v>
       </c>
+      <c r="AM68">
+        <f t="shared" si="3"/>
+        <v>0.64999999999999991</v>
+      </c>
+      <c r="AN68">
+        <f t="shared" si="2"/>
+        <v>6.74</v>
+      </c>
+      <c r="AO68">
+        <f t="shared" si="4"/>
+        <v>9.6439169139465861E-2</v>
+      </c>
     </row>
-    <row r="69" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -9274,8 +10113,20 @@
       <c r="AL69">
         <v>2</v>
       </c>
+      <c r="AM69">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AN69">
+        <f t="shared" si="2"/>
+        <v>3.7700000000000005</v>
+      </c>
+      <c r="AO69">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="70" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -9381,8 +10232,20 @@
       <c r="AL70">
         <v>1</v>
       </c>
+      <c r="AM70">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AN70">
+        <f t="shared" si="2"/>
+        <v>190.76</v>
+      </c>
+      <c r="AO70">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="71" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -9497,8 +10360,20 @@
       <c r="AL71">
         <v>1</v>
       </c>
+      <c r="AM71">
+        <f t="shared" si="3"/>
+        <v>190.76</v>
+      </c>
+      <c r="AN71">
+        <f t="shared" ref="AN71:AN134" si="5">ABS(SUM(9.24 - C71))</f>
+        <v>190.76</v>
+      </c>
+      <c r="AO71">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="72" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -9604,8 +10479,20 @@
       <c r="AL72">
         <v>2</v>
       </c>
+      <c r="AM72">
+        <f t="shared" si="3"/>
+        <v>4.24</v>
+      </c>
+      <c r="AN72">
+        <f t="shared" si="5"/>
+        <v>4.24</v>
+      </c>
+      <c r="AO72">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="73" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -9720,8 +10607,20 @@
       <c r="AL73">
         <v>2</v>
       </c>
+      <c r="AM73">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="AN73">
+        <f t="shared" si="5"/>
+        <v>7.24</v>
+      </c>
+      <c r="AO73">
+        <f t="shared" si="4"/>
+        <v>0.4143646408839779</v>
+      </c>
     </row>
-    <row r="74" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -9827,8 +10726,20 @@
       <c r="AL74">
         <v>2</v>
       </c>
+      <c r="AM74">
+        <f t="shared" si="3"/>
+        <v>140</v>
+      </c>
+      <c r="AN74">
+        <f t="shared" si="5"/>
+        <v>140.76</v>
+      </c>
+      <c r="AO74">
+        <f t="shared" si="4"/>
+        <v>0.99460073884626321</v>
+      </c>
     </row>
-    <row r="75" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -9934,8 +10845,20 @@
       <c r="AL75">
         <v>1</v>
       </c>
+      <c r="AM75">
+        <f t="shared" si="3"/>
+        <v>110.5</v>
+      </c>
+      <c r="AN75">
+        <f t="shared" si="5"/>
+        <v>110.76</v>
+      </c>
+      <c r="AO75">
+        <f t="shared" si="4"/>
+        <v>0.99765258215962438</v>
+      </c>
     </row>
-    <row r="76" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -10050,8 +10973,20 @@
       <c r="AL76">
         <v>2</v>
       </c>
+      <c r="AM76">
+        <f t="shared" si="3"/>
+        <v>0.2799999999999998</v>
+      </c>
+      <c r="AN76">
+        <f t="shared" si="5"/>
+        <v>6.74</v>
+      </c>
+      <c r="AO76">
+        <f t="shared" si="4"/>
+        <v>4.1543026706231424E-2</v>
+      </c>
     </row>
-    <row r="77" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -10166,8 +11101,20 @@
       <c r="AL77">
         <v>1</v>
       </c>
+      <c r="AM77">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="AN77">
+        <f t="shared" si="5"/>
+        <v>190.76</v>
+      </c>
+      <c r="AO77">
+        <f t="shared" si="4"/>
+        <v>0.26210945690920529</v>
+      </c>
     </row>
-    <row r="78" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -10282,8 +11229,20 @@
       <c r="AL78">
         <v>2</v>
       </c>
+      <c r="AM78">
+        <f t="shared" si="3"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="AN78">
+        <f t="shared" si="5"/>
+        <v>7.74</v>
+      </c>
+      <c r="AO78">
+        <f t="shared" si="4"/>
+        <v>3.8759689922480627E-2</v>
+      </c>
     </row>
-    <row r="79" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
@@ -10389,8 +11348,20 @@
       <c r="AL79">
         <v>1</v>
       </c>
+      <c r="AM79">
+        <f t="shared" si="3"/>
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="AN79">
+        <f t="shared" si="5"/>
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="AO79">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="80" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
@@ -10505,8 +11476,20 @@
       <c r="AL80">
         <v>2</v>
       </c>
+      <c r="AM80">
+        <f t="shared" si="3"/>
+        <v>5.1999999999999993</v>
+      </c>
+      <c r="AN80">
+        <f t="shared" si="5"/>
+        <v>5.24</v>
+      </c>
+      <c r="AO80">
+        <f t="shared" si="4"/>
+        <v>0.99236641221374033</v>
+      </c>
     </row>
-    <row r="81" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
@@ -10612,8 +11595,20 @@
       <c r="AL81">
         <v>2</v>
       </c>
+      <c r="AM81">
+        <f t="shared" si="3"/>
+        <v>1.7</v>
+      </c>
+      <c r="AN81">
+        <f t="shared" si="5"/>
+        <v>7.44</v>
+      </c>
+      <c r="AO81">
+        <f t="shared" si="4"/>
+        <v>0.22849462365591397</v>
+      </c>
     </row>
-    <row r="82" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
@@ -10719,8 +11714,20 @@
       <c r="AL82">
         <v>2</v>
       </c>
+      <c r="AM82">
+        <f t="shared" si="3"/>
+        <v>1.25</v>
+      </c>
+      <c r="AN82">
+        <f t="shared" si="5"/>
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="AO82">
+        <f t="shared" si="4"/>
+        <v>0.55803571428571419</v>
+      </c>
     </row>
-    <row r="83" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
@@ -10835,8 +11842,20 @@
       <c r="AL83">
         <v>2</v>
       </c>
+      <c r="AM83">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AN83">
+        <f t="shared" si="5"/>
+        <v>7.24</v>
+      </c>
+      <c r="AO83">
+        <f t="shared" si="4"/>
+        <v>0.13812154696132597</v>
+      </c>
     </row>
-    <row r="84" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
@@ -10942,8 +11961,20 @@
       <c r="AL84">
         <v>2</v>
       </c>
+      <c r="AM84">
+        <f t="shared" si="3"/>
+        <v>2.6799999999999997</v>
+      </c>
+      <c r="AN84">
+        <f t="shared" si="5"/>
+        <v>4.24</v>
+      </c>
+      <c r="AO84">
+        <f t="shared" si="4"/>
+        <v>0.63207547169811307</v>
+      </c>
     </row>
-    <row r="85" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
@@ -11058,8 +12089,20 @@
       <c r="AL85">
         <v>2</v>
       </c>
+      <c r="AM85">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AN85">
+        <f t="shared" si="5"/>
+        <v>6.24</v>
+      </c>
+      <c r="AO85">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="86" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
@@ -11165,8 +12208,20 @@
       <c r="AL86">
         <v>1</v>
       </c>
+      <c r="AM86">
+        <f t="shared" si="3"/>
+        <v>290</v>
+      </c>
+      <c r="AN86">
+        <f t="shared" si="5"/>
+        <v>290.76</v>
+      </c>
+      <c r="AO86">
+        <f t="shared" si="4"/>
+        <v>0.99738616040720873</v>
+      </c>
     </row>
-    <row r="87" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
@@ -11281,8 +12336,20 @@
       <c r="AL87">
         <v>1</v>
       </c>
+      <c r="AM87">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AN87">
+        <f t="shared" si="5"/>
+        <v>140.76</v>
+      </c>
+      <c r="AO87">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="88" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
@@ -11397,8 +12464,20 @@
       <c r="AL88">
         <v>2</v>
       </c>
+      <c r="AM88">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="AN88">
+        <f t="shared" si="5"/>
+        <v>6.24</v>
+      </c>
+      <c r="AO88">
+        <f t="shared" si="4"/>
+        <v>0.32051282051282048</v>
+      </c>
     </row>
-    <row r="89" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
@@ -11513,8 +12592,20 @@
       <c r="AL89">
         <v>1</v>
       </c>
+      <c r="AM89">
+        <f t="shared" si="3"/>
+        <v>240.76</v>
+      </c>
+      <c r="AN89">
+        <f t="shared" si="5"/>
+        <v>240.76</v>
+      </c>
+      <c r="AO89">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="90" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>89</v>
       </c>
@@ -11620,8 +12711,20 @@
       <c r="AL90">
         <v>1</v>
       </c>
+      <c r="AM90">
+        <f t="shared" si="3"/>
+        <v>240</v>
+      </c>
+      <c r="AN90">
+        <f t="shared" si="5"/>
+        <v>240.76</v>
+      </c>
+      <c r="AO90">
+        <f t="shared" si="4"/>
+        <v>0.99684332945672038</v>
+      </c>
     </row>
-    <row r="91" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>90</v>
       </c>
@@ -11727,8 +12830,20 @@
       <c r="AL91">
         <v>1</v>
       </c>
+      <c r="AM91">
+        <f t="shared" si="3"/>
+        <v>477.5</v>
+      </c>
+      <c r="AN91">
+        <f t="shared" si="5"/>
+        <v>470.76</v>
+      </c>
+      <c r="AO91">
+        <f t="shared" si="4"/>
+        <v>1.0143172741949189</v>
+      </c>
     </row>
-    <row r="92" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
@@ -11834,8 +12949,20 @@
       <c r="AL92">
         <v>2</v>
       </c>
+      <c r="AM92">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="AN92">
+        <f t="shared" si="5"/>
+        <v>6.24</v>
+      </c>
+      <c r="AO92">
+        <f t="shared" si="4"/>
+        <v>0.96153846153846145</v>
+      </c>
     </row>
-    <row r="93" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
@@ -11950,8 +13077,20 @@
       <c r="AL93">
         <v>1</v>
       </c>
+      <c r="AM93">
+        <f t="shared" si="3"/>
+        <v>490.76</v>
+      </c>
+      <c r="AN93">
+        <f t="shared" si="5"/>
+        <v>490.76</v>
+      </c>
+      <c r="AO93">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="94" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
@@ -12066,8 +13205,20 @@
       <c r="AL94">
         <v>1</v>
       </c>
+      <c r="AM94">
+        <f t="shared" si="3"/>
+        <v>8.24</v>
+      </c>
+      <c r="AN94">
+        <f t="shared" si="5"/>
+        <v>8.24</v>
+      </c>
+      <c r="AO94">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="95" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
@@ -12173,8 +13324,20 @@
       <c r="AL95">
         <v>1</v>
       </c>
+      <c r="AM95">
+        <f t="shared" si="3"/>
+        <v>1.5</v>
+      </c>
+      <c r="AN95">
+        <f t="shared" si="5"/>
+        <v>6.24</v>
+      </c>
+      <c r="AO95">
+        <f t="shared" si="4"/>
+        <v>0.24038461538461536</v>
+      </c>
     </row>
-    <row r="96" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
       </c>
@@ -12280,8 +13443,20 @@
       <c r="AL96">
         <v>1</v>
       </c>
+      <c r="AM96">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="AN96">
+        <f t="shared" si="5"/>
+        <v>60.76</v>
+      </c>
+      <c r="AO96">
+        <f t="shared" si="4"/>
+        <v>0.9874917709019092</v>
+      </c>
     </row>
-    <row r="97" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>96</v>
       </c>
@@ -12387,8 +13562,20 @@
       <c r="AL97">
         <v>1</v>
       </c>
+      <c r="AM97">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AN97">
+        <f t="shared" si="5"/>
+        <v>190.76</v>
+      </c>
+      <c r="AO97">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="98" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>97</v>
       </c>
@@ -12494,8 +13681,20 @@
       <c r="AL98">
         <v>2</v>
       </c>
+      <c r="AM98">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AN98">
+        <f t="shared" si="5"/>
+        <v>4.74</v>
+      </c>
+      <c r="AO98">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="99" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>98</v>
       </c>
@@ -12601,8 +13800,20 @@
       <c r="AL99">
         <v>2</v>
       </c>
+      <c r="AM99">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="AN99">
+        <f t="shared" si="5"/>
+        <v>4.76</v>
+      </c>
+      <c r="AO99">
+        <f t="shared" si="4"/>
+        <v>0.84033613445378152</v>
+      </c>
     </row>
-    <row r="100" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>99</v>
       </c>
@@ -12708,8 +13919,20 @@
       <c r="AL100">
         <v>1</v>
       </c>
+      <c r="AM100">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="AN100">
+        <f t="shared" si="5"/>
+        <v>40.76</v>
+      </c>
+      <c r="AO100">
+        <f t="shared" si="4"/>
+        <v>0.98135426889106969</v>
+      </c>
     </row>
-    <row r="101" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>100</v>
       </c>
@@ -12815,8 +14038,20 @@
       <c r="AL101">
         <v>2</v>
       </c>
+      <c r="AM101">
+        <f t="shared" si="3"/>
+        <v>5.49</v>
+      </c>
+      <c r="AN101">
+        <f t="shared" si="5"/>
+        <v>5.49</v>
+      </c>
+      <c r="AO101">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="102" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>101</v>
       </c>
@@ -12931,8 +14166,20 @@
       <c r="AL102">
         <v>1</v>
       </c>
+      <c r="AM102">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="AN102">
+        <f t="shared" si="5"/>
+        <v>490.76</v>
+      </c>
+      <c r="AO102">
+        <f t="shared" si="4"/>
+        <v>0.10188279403374359</v>
+      </c>
     </row>
-    <row r="103" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>102</v>
       </c>
@@ -13038,8 +14285,20 @@
       <c r="AL103">
         <v>2</v>
       </c>
+      <c r="AM103">
+        <f t="shared" si="3"/>
+        <v>0.12000000000000011</v>
+      </c>
+      <c r="AN103">
+        <f t="shared" si="5"/>
+        <v>7.24</v>
+      </c>
+      <c r="AO103">
+        <f t="shared" si="4"/>
+        <v>1.6574585635359129E-2</v>
+      </c>
     </row>
-    <row r="104" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>103</v>
       </c>
@@ -13145,8 +14404,20 @@
       <c r="AL104">
         <v>1</v>
       </c>
+      <c r="AM104">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="AN104">
+        <f t="shared" si="5"/>
+        <v>40.76</v>
+      </c>
+      <c r="AO104">
+        <f t="shared" si="4"/>
+        <v>0.98135426889106969</v>
+      </c>
     </row>
-    <row r="105" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>104</v>
       </c>
@@ -13252,8 +14523,20 @@
       <c r="AL105">
         <v>1</v>
       </c>
+      <c r="AM105">
+        <f t="shared" si="3"/>
+        <v>300</v>
+      </c>
+      <c r="AN105">
+        <f t="shared" si="5"/>
+        <v>340.76</v>
+      </c>
+      <c r="AO105">
+        <f t="shared" si="4"/>
+        <v>0.88038502171616384</v>
+      </c>
     </row>
-    <row r="106" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>105</v>
       </c>
@@ -13368,8 +14651,20 @@
       <c r="AL106">
         <v>2</v>
       </c>
+      <c r="AM106">
+        <f t="shared" si="3"/>
+        <v>5.87</v>
+      </c>
+      <c r="AN106">
+        <f t="shared" si="5"/>
+        <v>6.87</v>
+      </c>
+      <c r="AO106">
+        <f t="shared" si="4"/>
+        <v>0.85443959243085876</v>
+      </c>
     </row>
-    <row r="107" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>106</v>
       </c>
@@ -13475,8 +14770,20 @@
       <c r="AL107">
         <v>2</v>
       </c>
+      <c r="AM107">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AN107">
+        <f t="shared" si="5"/>
+        <v>4.24</v>
+      </c>
+      <c r="AO107">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="108" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>107</v>
       </c>
@@ -13582,8 +14889,20 @@
       <c r="AL108">
         <v>2</v>
       </c>
+      <c r="AM108">
+        <f t="shared" si="3"/>
+        <v>1.75</v>
+      </c>
+      <c r="AN108">
+        <f t="shared" si="5"/>
+        <v>5.99</v>
+      </c>
+      <c r="AO108">
+        <f t="shared" si="4"/>
+        <v>0.29215358931552587</v>
+      </c>
     </row>
-    <row r="109" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>108</v>
       </c>
@@ -13689,8 +15008,20 @@
       <c r="AL109">
         <v>1</v>
       </c>
+      <c r="AM109">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="AN109">
+        <f t="shared" si="5"/>
+        <v>10.76</v>
+      </c>
+      <c r="AO109">
+        <f t="shared" si="4"/>
+        <v>0.46468401486988847</v>
+      </c>
     </row>
-    <row r="110" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>109</v>
       </c>
@@ -13796,8 +15127,20 @@
       <c r="AL110">
         <v>1</v>
       </c>
+      <c r="AM110">
+        <f t="shared" si="3"/>
+        <v>90.5</v>
+      </c>
+      <c r="AN110">
+        <f t="shared" si="5"/>
+        <v>90.76</v>
+      </c>
+      <c r="AO110">
+        <f t="shared" si="4"/>
+        <v>0.99713530189510791</v>
+      </c>
     </row>
-    <row r="111" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>110</v>
       </c>
@@ -13912,8 +15255,20 @@
       <c r="AL111">
         <v>1</v>
       </c>
+      <c r="AM111">
+        <f t="shared" si="3"/>
+        <v>140</v>
+      </c>
+      <c r="AN111">
+        <f t="shared" si="5"/>
+        <v>140.76</v>
+      </c>
+      <c r="AO111">
+        <f t="shared" si="4"/>
+        <v>0.99460073884626321</v>
+      </c>
     </row>
-    <row r="112" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>111</v>
       </c>
@@ -14019,8 +15374,20 @@
       <c r="AL112">
         <v>2</v>
       </c>
+      <c r="AM112">
+        <f t="shared" si="3"/>
+        <v>0.24000000000000021</v>
+      </c>
+      <c r="AN112">
+        <f t="shared" si="5"/>
+        <v>6.0600000000000005</v>
+      </c>
+      <c r="AO112">
+        <f t="shared" si="4"/>
+        <v>3.9603960396039639E-2</v>
+      </c>
     </row>
-    <row r="113" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>112</v>
       </c>
@@ -14135,8 +15502,20 @@
       <c r="AL113">
         <v>1</v>
       </c>
+      <c r="AM113">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AN113">
+        <f t="shared" si="5"/>
+        <v>890.76</v>
+      </c>
+      <c r="AO113">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="114" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>113</v>
       </c>
@@ -14242,8 +15621,19 @@
       <c r="AL114">
         <v>1</v>
       </c>
+      <c r="AM114">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AN114">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AO114">
+        <v>99</v>
+      </c>
     </row>
-    <row r="115" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>114</v>
       </c>
@@ -14349,8 +15739,20 @@
       <c r="AL115">
         <v>1</v>
       </c>
+      <c r="AM115">
+        <f t="shared" si="3"/>
+        <v>290.76</v>
+      </c>
+      <c r="AN115">
+        <f t="shared" si="5"/>
+        <v>290.76</v>
+      </c>
+      <c r="AO115">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="116" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>115</v>
       </c>
@@ -14456,8 +15858,20 @@
       <c r="AL116">
         <v>1</v>
       </c>
+      <c r="AM116">
+        <f t="shared" si="3"/>
+        <v>292</v>
+      </c>
+      <c r="AN116">
+        <f t="shared" si="5"/>
+        <v>290.76</v>
+      </c>
+      <c r="AO116">
+        <f t="shared" si="4"/>
+        <v>1.0042646856513964</v>
+      </c>
     </row>
-    <row r="117" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>116</v>
       </c>
@@ -14572,8 +15986,20 @@
       <c r="AL117">
         <v>2</v>
       </c>
+      <c r="AM117">
+        <f t="shared" si="3"/>
+        <v>1.2400000000000002</v>
+      </c>
+      <c r="AN117">
+        <f t="shared" si="5"/>
+        <v>1.2400000000000002</v>
+      </c>
+      <c r="AO117">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="118" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>117</v>
       </c>
@@ -14679,8 +16105,20 @@
       <c r="AL118">
         <v>2</v>
       </c>
+      <c r="AM118">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AN118">
+        <f t="shared" si="5"/>
+        <v>6.24</v>
+      </c>
+      <c r="AO118">
+        <f t="shared" si="4"/>
+        <v>0.16025641025641024</v>
+      </c>
     </row>
-    <row r="119" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>118</v>
       </c>
@@ -14786,8 +16224,20 @@
       <c r="AL119">
         <v>2</v>
       </c>
+      <c r="AM119">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="AN119">
+        <f t="shared" si="5"/>
+        <v>4.24</v>
+      </c>
+      <c r="AO119">
+        <f t="shared" si="4"/>
+        <v>0.47169811320754712</v>
+      </c>
     </row>
-    <row r="120" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>119</v>
       </c>
@@ -14902,8 +16352,20 @@
       <c r="AL120">
         <v>1</v>
       </c>
+      <c r="AM120">
+        <f t="shared" si="3"/>
+        <v>190</v>
+      </c>
+      <c r="AN120">
+        <f t="shared" si="5"/>
+        <v>190.76</v>
+      </c>
+      <c r="AO120">
+        <f t="shared" si="4"/>
+        <v>0.99601593625498008</v>
+      </c>
     </row>
-    <row r="121" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>120</v>
       </c>
@@ -15009,8 +16471,20 @@
       <c r="AL121">
         <v>2</v>
       </c>
+      <c r="AM121">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="AN121">
+        <f t="shared" si="5"/>
+        <v>3.74</v>
+      </c>
+      <c r="AO121">
+        <f t="shared" si="4"/>
+        <v>0.53475935828876997</v>
+      </c>
     </row>
-    <row r="122" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>121</v>
       </c>
@@ -15125,8 +16599,20 @@
       <c r="AL122">
         <v>1</v>
       </c>
+      <c r="AM122">
+        <f t="shared" si="3"/>
+        <v>190.5</v>
+      </c>
+      <c r="AN122">
+        <f t="shared" si="5"/>
+        <v>190.76</v>
+      </c>
+      <c r="AO122">
+        <f t="shared" si="4"/>
+        <v>0.99863703082407218</v>
+      </c>
     </row>
-    <row r="123" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>122</v>
       </c>
@@ -15232,8 +16718,20 @@
       <c r="AL123">
         <v>2</v>
       </c>
+      <c r="AM123">
+        <f t="shared" si="3"/>
+        <v>2.25</v>
+      </c>
+      <c r="AN123">
+        <f t="shared" si="5"/>
+        <v>4.74</v>
+      </c>
+      <c r="AO123">
+        <f t="shared" si="4"/>
+        <v>0.47468354430379744</v>
+      </c>
     </row>
-    <row r="124" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>123</v>
       </c>
@@ -15339,8 +16837,20 @@
       <c r="AL124">
         <v>2</v>
       </c>
+      <c r="AM124">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AN124">
+        <f t="shared" si="5"/>
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="AO124">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="125" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>124</v>
       </c>
@@ -15455,8 +16965,20 @@
       <c r="AL125">
         <v>2</v>
       </c>
+      <c r="AM125">
+        <f t="shared" si="3"/>
+        <v>4.24</v>
+      </c>
+      <c r="AN125">
+        <f t="shared" si="5"/>
+        <v>4.24</v>
+      </c>
+      <c r="AO125">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="126" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>125</v>
       </c>
@@ -15571,8 +17093,20 @@
       <c r="AL126">
         <v>1</v>
       </c>
+      <c r="AM126">
+        <f t="shared" si="3"/>
+        <v>150</v>
+      </c>
+      <c r="AN126">
+        <f t="shared" si="5"/>
+        <v>190.76</v>
+      </c>
+      <c r="AO126">
+        <f t="shared" si="4"/>
+        <v>0.78632837072761586</v>
+      </c>
     </row>
-    <row r="127" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>126</v>
       </c>
@@ -15678,8 +17212,20 @@
       <c r="AL127">
         <v>1</v>
       </c>
+      <c r="AM127">
+        <f t="shared" si="3"/>
+        <v>849</v>
+      </c>
+      <c r="AN127">
+        <f t="shared" si="5"/>
+        <v>889.76</v>
+      </c>
+      <c r="AO127">
+        <f t="shared" si="4"/>
+        <v>0.95418989390397413</v>
+      </c>
     </row>
-    <row r="128" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>127</v>
       </c>
@@ -15794,8 +17340,20 @@
       <c r="AL128">
         <v>2</v>
       </c>
+      <c r="AM128">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="AN128">
+        <f t="shared" si="5"/>
+        <v>5.24</v>
+      </c>
+      <c r="AO128">
+        <f t="shared" si="4"/>
+        <v>0.38167938931297707</v>
+      </c>
     </row>
-    <row r="129" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>128</v>
       </c>
@@ -15901,8 +17459,20 @@
       <c r="AL129">
         <v>2</v>
       </c>
+      <c r="AM129">
+        <f t="shared" si="3"/>
+        <v>2.6</v>
+      </c>
+      <c r="AN129">
+        <f t="shared" si="5"/>
+        <v>7.84</v>
+      </c>
+      <c r="AO129">
+        <f t="shared" si="4"/>
+        <v>0.33163265306122452</v>
+      </c>
     </row>
-    <row r="130" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>129</v>
       </c>
@@ -16017,8 +17587,20 @@
       <c r="AL130">
         <v>1</v>
       </c>
+      <c r="AM130">
+        <f t="shared" si="3"/>
+        <v>900</v>
+      </c>
+      <c r="AN130">
+        <f t="shared" si="5"/>
+        <v>990.76</v>
+      </c>
+      <c r="AO130">
+        <f t="shared" si="4"/>
+        <v>0.90839355646170616</v>
+      </c>
     </row>
-    <row r="131" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>130</v>
       </c>
@@ -16124,8 +17706,20 @@
       <c r="AL131">
         <v>2</v>
       </c>
+      <c r="AM131">
+        <f t="shared" ref="AM131:AM194" si="6">ABS(SUM(AE131-C131))</f>
+        <v>1.5</v>
+      </c>
+      <c r="AN131">
+        <f t="shared" si="5"/>
+        <v>5.74</v>
+      </c>
+      <c r="AO131">
+        <f t="shared" ref="AO131:AO194" si="7">SUM(AM131/AN131)</f>
+        <v>0.26132404181184671</v>
+      </c>
     </row>
-    <row r="132" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>131</v>
       </c>
@@ -16240,8 +17834,20 @@
       <c r="AL132">
         <v>2</v>
       </c>
+      <c r="AM132">
+        <f t="shared" si="6"/>
+        <v>3.24</v>
+      </c>
+      <c r="AN132">
+        <f t="shared" si="5"/>
+        <v>3.24</v>
+      </c>
+      <c r="AO132">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="133" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>132</v>
       </c>
@@ -16347,8 +17953,20 @@
       <c r="AL133">
         <v>2</v>
       </c>
+      <c r="AM133">
+        <f t="shared" si="6"/>
+        <v>296.5</v>
+      </c>
+      <c r="AN133">
+        <f t="shared" si="5"/>
+        <v>290.76</v>
+      </c>
+      <c r="AO133">
+        <f t="shared" si="7"/>
+        <v>1.0197413674508187</v>
+      </c>
     </row>
-    <row r="134" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>133</v>
       </c>
@@ -16454,8 +18072,20 @@
       <c r="AL134">
         <v>1</v>
       </c>
+      <c r="AM134">
+        <f t="shared" si="6"/>
+        <v>450</v>
+      </c>
+      <c r="AN134">
+        <f t="shared" si="5"/>
+        <v>490.76</v>
+      </c>
+      <c r="AO134">
+        <f t="shared" si="7"/>
+        <v>0.91694514630369228</v>
+      </c>
     </row>
-    <row r="135" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>134</v>
       </c>
@@ -16561,8 +18191,20 @@
       <c r="AL135">
         <v>2</v>
       </c>
+      <c r="AM135">
+        <f t="shared" si="6"/>
+        <v>0.39999999999999991</v>
+      </c>
+      <c r="AN135">
+        <f t="shared" ref="AN135:AN197" si="8">ABS(SUM(9.24 - C135))</f>
+        <v>7.65</v>
+      </c>
+      <c r="AO135">
+        <f t="shared" si="7"/>
+        <v>5.2287581699346393E-2</v>
+      </c>
     </row>
-    <row r="136" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>135</v>
       </c>
@@ -16668,8 +18310,20 @@
       <c r="AL136">
         <v>1</v>
       </c>
+      <c r="AM136">
+        <f t="shared" si="6"/>
+        <v>5.05</v>
+      </c>
+      <c r="AN136">
+        <f t="shared" si="8"/>
+        <v>8.2900000000000009</v>
+      </c>
+      <c r="AO136">
+        <f t="shared" si="7"/>
+        <v>0.60916767189384791</v>
+      </c>
     </row>
-    <row r="137" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>136</v>
       </c>
@@ -16784,8 +18438,20 @@
       <c r="AL137">
         <v>2</v>
       </c>
+      <c r="AM137">
+        <f t="shared" si="6"/>
+        <v>1.25</v>
+      </c>
+      <c r="AN137">
+        <f t="shared" si="8"/>
+        <v>5.99</v>
+      </c>
+      <c r="AO137">
+        <f t="shared" si="7"/>
+        <v>0.20868113522537562</v>
+      </c>
     </row>
-    <row r="138" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>137</v>
       </c>
@@ -16891,8 +18557,20 @@
       <c r="AL138">
         <v>1</v>
       </c>
+      <c r="AM138">
+        <f t="shared" si="6"/>
+        <v>5.74</v>
+      </c>
+      <c r="AN138">
+        <f t="shared" si="8"/>
+        <v>5.74</v>
+      </c>
+      <c r="AO138">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="139" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>138</v>
       </c>
@@ -16998,8 +18676,20 @@
       <c r="AL139">
         <v>1</v>
       </c>
+      <c r="AM139">
+        <f t="shared" si="6"/>
+        <v>140.5</v>
+      </c>
+      <c r="AN139">
+        <f t="shared" si="8"/>
+        <v>140.76</v>
+      </c>
+      <c r="AO139">
+        <f t="shared" si="7"/>
+        <v>0.99815288434214267</v>
+      </c>
     </row>
-    <row r="140" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>139</v>
       </c>
@@ -17105,8 +18795,20 @@
       <c r="AL140">
         <v>1</v>
       </c>
+      <c r="AM140">
+        <f t="shared" si="6"/>
+        <v>240.75</v>
+      </c>
+      <c r="AN140">
+        <f t="shared" si="8"/>
+        <v>240.76</v>
+      </c>
+      <c r="AO140">
+        <f t="shared" si="7"/>
+        <v>0.99995846486127271</v>
+      </c>
     </row>
-    <row r="141" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>140</v>
       </c>
@@ -17212,8 +18914,20 @@
       <c r="AL141">
         <v>2</v>
       </c>
+      <c r="AM141">
+        <f t="shared" si="6"/>
+        <v>1.5</v>
+      </c>
+      <c r="AN141">
+        <f t="shared" si="8"/>
+        <v>7.24</v>
+      </c>
+      <c r="AO141">
+        <f t="shared" si="7"/>
+        <v>0.20718232044198895</v>
+      </c>
     </row>
-    <row r="142" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>141</v>
       </c>
@@ -17328,8 +19042,20 @@
       <c r="AL142">
         <v>2</v>
       </c>
+      <c r="AM142">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AN142">
+        <f t="shared" si="8"/>
+        <v>5.24</v>
+      </c>
+      <c r="AO142">
+        <f t="shared" si="7"/>
+        <v>0.19083969465648853</v>
+      </c>
     </row>
-    <row r="143" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>142</v>
       </c>
@@ -17435,8 +19161,20 @@
       <c r="AL143">
         <v>2</v>
       </c>
+      <c r="AM143">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="AN143">
+        <f t="shared" si="8"/>
+        <v>7.24</v>
+      </c>
+      <c r="AO143">
+        <f t="shared" si="7"/>
+        <v>6.9060773480662987E-2</v>
+      </c>
     </row>
-    <row r="144" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>143</v>
       </c>
@@ -17542,8 +19280,20 @@
       <c r="AL144">
         <v>1</v>
       </c>
+      <c r="AM144">
+        <f t="shared" si="6"/>
+        <v>290.75</v>
+      </c>
+      <c r="AN144">
+        <f t="shared" si="8"/>
+        <v>290.76</v>
+      </c>
+      <c r="AO144">
+        <f t="shared" si="7"/>
+        <v>0.99996560737377904</v>
+      </c>
     </row>
-    <row r="145" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>144</v>
       </c>
@@ -17658,8 +19408,20 @@
       <c r="AL145">
         <v>1</v>
       </c>
+      <c r="AM145">
+        <f t="shared" si="6"/>
+        <v>482.76</v>
+      </c>
+      <c r="AN145">
+        <f t="shared" si="8"/>
+        <v>482.76</v>
+      </c>
+      <c r="AO145">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="146" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>145</v>
       </c>
@@ -17765,8 +19527,20 @@
       <c r="AL146">
         <v>2</v>
       </c>
+      <c r="AM146">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AN146">
+        <f t="shared" si="8"/>
+        <v>5.74</v>
+      </c>
+      <c r="AO146">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="147" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>146</v>
       </c>
@@ -17872,8 +19646,20 @@
       <c r="AL147">
         <v>1</v>
       </c>
+      <c r="AM147">
+        <f t="shared" si="6"/>
+        <v>100</v>
+      </c>
+      <c r="AN147">
+        <f t="shared" si="8"/>
+        <v>90.76</v>
+      </c>
+      <c r="AO147">
+        <f t="shared" si="7"/>
+        <v>1.1018069634200087</v>
+      </c>
     </row>
-    <row r="148" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>147</v>
       </c>
@@ -17988,8 +19774,20 @@
       <c r="AL148">
         <v>1</v>
       </c>
+      <c r="AM148">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="AN148">
+        <f t="shared" si="8"/>
+        <v>18.759999999999998</v>
+      </c>
+      <c r="AO148">
+        <f t="shared" si="7"/>
+        <v>0.63965884861407252</v>
+      </c>
     </row>
-    <row r="149" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>148</v>
       </c>
@@ -18095,8 +19893,20 @@
       <c r="AL149">
         <v>2</v>
       </c>
+      <c r="AM149">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="AN149">
+        <f t="shared" si="8"/>
+        <v>6.24</v>
+      </c>
+      <c r="AO149">
+        <f t="shared" si="7"/>
+        <v>0.64102564102564097</v>
+      </c>
     </row>
-    <row r="150" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>149</v>
       </c>
@@ -18202,8 +20012,20 @@
       <c r="AL150">
         <v>1</v>
       </c>
+      <c r="AM150">
+        <f t="shared" si="6"/>
+        <v>50</v>
+      </c>
+      <c r="AN150">
+        <f t="shared" si="8"/>
+        <v>140.76</v>
+      </c>
+      <c r="AO150">
+        <f t="shared" si="7"/>
+        <v>0.35521454958795112</v>
+      </c>
     </row>
-    <row r="151" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>150</v>
       </c>
@@ -18309,8 +20131,20 @@
       <c r="AL151">
         <v>1</v>
       </c>
+      <c r="AM151">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AN151">
+        <f t="shared" si="8"/>
+        <v>290.76</v>
+      </c>
+      <c r="AO151">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="152" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>151</v>
       </c>
@@ -18416,8 +20250,20 @@
       <c r="AL152">
         <v>2</v>
       </c>
+      <c r="AM152">
+        <f t="shared" si="6"/>
+        <v>100</v>
+      </c>
+      <c r="AN152">
+        <f t="shared" si="8"/>
+        <v>140.76</v>
+      </c>
+      <c r="AO152">
+        <f t="shared" si="7"/>
+        <v>0.71042909917590225</v>
+      </c>
     </row>
-    <row r="153" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>152</v>
       </c>
@@ -18532,8 +20378,20 @@
       <c r="AL153">
         <v>2</v>
       </c>
+      <c r="AM153">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="AN153">
+        <f t="shared" si="8"/>
+        <v>4.24</v>
+      </c>
+      <c r="AO153">
+        <f t="shared" si="7"/>
+        <v>0.94339622641509424</v>
+      </c>
     </row>
-    <row r="154" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:41" ht="306" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>153</v>
       </c>
@@ -18639,8 +20497,20 @@
       <c r="AL154">
         <v>1</v>
       </c>
+      <c r="AM154">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AN154">
+        <f t="shared" si="8"/>
+        <v>245.76</v>
+      </c>
+      <c r="AO154">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="155" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>154</v>
       </c>
@@ -18746,8 +20616,20 @@
       <c r="AL155">
         <v>1</v>
       </c>
+      <c r="AM155">
+        <f t="shared" si="6"/>
+        <v>44</v>
+      </c>
+      <c r="AN155">
+        <f t="shared" si="8"/>
+        <v>45.76</v>
+      </c>
+      <c r="AO155">
+        <f t="shared" si="7"/>
+        <v>0.96153846153846156</v>
+      </c>
     </row>
-    <row r="156" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:41" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>155</v>
       </c>
@@ -18853,8 +20735,20 @@
       <c r="AL156">
         <v>1</v>
       </c>
+      <c r="AM156">
+        <f t="shared" si="6"/>
+        <v>204</v>
+      </c>
+      <c r="AN156">
+        <f t="shared" si="8"/>
+        <v>203.76</v>
+      </c>
+      <c r="AO156">
+        <f t="shared" si="7"/>
+        <v>1.0011778563015312</v>
+      </c>
     </row>
-    <row r="157" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>156</v>
       </c>
@@ -18960,8 +20854,20 @@
       <c r="AL157">
         <v>1</v>
       </c>
+      <c r="AM157">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AN157">
+        <f t="shared" si="8"/>
+        <v>190.76</v>
+      </c>
+      <c r="AO157">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="158" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>157</v>
       </c>
@@ -19076,8 +20982,20 @@
       <c r="AL158">
         <v>1</v>
       </c>
+      <c r="AM158">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AN158">
+        <f t="shared" si="8"/>
+        <v>190.76</v>
+      </c>
+      <c r="AO158">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="159" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:41" ht="306" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>158</v>
       </c>
@@ -19183,8 +21101,20 @@
       <c r="AL159">
         <v>1</v>
       </c>
+      <c r="AM159">
+        <f t="shared" si="6"/>
+        <v>55</v>
+      </c>
+      <c r="AN159">
+        <f t="shared" si="8"/>
+        <v>290.76</v>
+      </c>
+      <c r="AO159">
+        <f t="shared" si="7"/>
+        <v>0.18915944421516029</v>
+      </c>
     </row>
-    <row r="160" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>159</v>
       </c>
@@ -19290,8 +21220,20 @@
       <c r="AL160">
         <v>1</v>
       </c>
+      <c r="AM160">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AN160">
+        <f t="shared" si="8"/>
+        <v>1.2400000000000002</v>
+      </c>
+      <c r="AO160">
+        <f t="shared" si="7"/>
+        <v>0.80645161290322565</v>
+      </c>
     </row>
-    <row r="161" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>160</v>
       </c>
@@ -19406,8 +21348,20 @@
       <c r="AL161">
         <v>2</v>
       </c>
+      <c r="AM161">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="AN161">
+        <f t="shared" si="8"/>
+        <v>90.76</v>
+      </c>
+      <c r="AO161">
+        <f t="shared" si="7"/>
+        <v>0.11018069634200088</v>
+      </c>
     </row>
-    <row r="162" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>161</v>
       </c>
@@ -19513,8 +21467,20 @@
       <c r="AL162">
         <v>1</v>
       </c>
+      <c r="AM162">
+        <f t="shared" si="6"/>
+        <v>500</v>
+      </c>
+      <c r="AN162">
+        <f t="shared" si="8"/>
+        <v>990.76</v>
+      </c>
+      <c r="AO162">
+        <f t="shared" si="7"/>
+        <v>0.50466308692317008</v>
+      </c>
     </row>
-    <row r="163" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>162</v>
       </c>
@@ -19620,8 +21586,20 @@
       <c r="AL163">
         <v>2</v>
       </c>
+      <c r="AM163">
+        <f t="shared" si="6"/>
+        <v>1.25</v>
+      </c>
+      <c r="AN163">
+        <f t="shared" si="8"/>
+        <v>7.49</v>
+      </c>
+      <c r="AO163">
+        <f t="shared" si="7"/>
+        <v>0.16688918558077437</v>
+      </c>
     </row>
-    <row r="164" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:41" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>163</v>
       </c>
@@ -19727,8 +21705,20 @@
       <c r="AL164">
         <v>1</v>
       </c>
+      <c r="AM164">
+        <f t="shared" si="6"/>
+        <v>0.24000000000000021</v>
+      </c>
+      <c r="AN164">
+        <f t="shared" si="8"/>
+        <v>0.25</v>
+      </c>
+      <c r="AO164">
+        <f t="shared" si="7"/>
+        <v>0.96000000000000085</v>
+      </c>
     </row>
-    <row r="165" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:41" ht="34" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>164</v>
       </c>
@@ -19834,8 +21824,20 @@
       <c r="AL165">
         <v>1</v>
       </c>
+      <c r="AM165">
+        <f t="shared" si="6"/>
+        <v>101</v>
+      </c>
+      <c r="AN165">
+        <f t="shared" si="8"/>
+        <v>345.76</v>
+      </c>
+      <c r="AO165">
+        <f t="shared" si="7"/>
+        <v>0.29211013419713094</v>
+      </c>
     </row>
-    <row r="166" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:41" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>165</v>
       </c>
@@ -19941,8 +21943,20 @@
       <c r="AL166">
         <v>1</v>
       </c>
+      <c r="AM166">
+        <f t="shared" si="6"/>
+        <v>0.24000000000000021</v>
+      </c>
+      <c r="AN166">
+        <f t="shared" si="8"/>
+        <v>0.24000000000000021</v>
+      </c>
+      <c r="AO166">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="167" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>166</v>
       </c>
@@ -20048,8 +22062,20 @@
       <c r="AL167">
         <v>1</v>
       </c>
+      <c r="AM167">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AN167">
+        <f t="shared" si="8"/>
+        <v>190.76</v>
+      </c>
+      <c r="AO167">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="168" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>167</v>
       </c>
@@ -20155,8 +22181,20 @@
       <c r="AL168">
         <v>1</v>
       </c>
+      <c r="AM168">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AN168">
+        <f t="shared" si="8"/>
+        <v>190.76</v>
+      </c>
+      <c r="AO168">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="169" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>168</v>
       </c>
@@ -20262,8 +22300,20 @@
       <c r="AL169">
         <v>2</v>
       </c>
+      <c r="AM169">
+        <f t="shared" si="6"/>
+        <v>100</v>
+      </c>
+      <c r="AN169">
+        <f t="shared" si="8"/>
+        <v>240.76</v>
+      </c>
+      <c r="AO169">
+        <f t="shared" si="7"/>
+        <v>0.41535138727363352</v>
+      </c>
     </row>
-    <row r="170" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>169</v>
       </c>
@@ -20369,8 +22419,20 @@
       <c r="AL170">
         <v>1</v>
       </c>
+      <c r="AM170">
+        <f t="shared" si="6"/>
+        <v>100</v>
+      </c>
+      <c r="AN170">
+        <f t="shared" si="8"/>
+        <v>280.76</v>
+      </c>
+      <c r="AO170">
+        <f t="shared" si="7"/>
+        <v>0.35617609346060691</v>
+      </c>
     </row>
-    <row r="171" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>170</v>
       </c>
@@ -20476,8 +22538,20 @@
       <c r="AL171">
         <v>2</v>
       </c>
+      <c r="AM171">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AN171">
+        <f t="shared" si="8"/>
+        <v>3.3900000000000006</v>
+      </c>
+      <c r="AO171">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="172" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>171</v>
       </c>
@@ -20583,8 +22657,20 @@
       <c r="AL172">
         <v>1</v>
       </c>
+      <c r="AM172">
+        <f t="shared" si="6"/>
+        <v>66</v>
+      </c>
+      <c r="AN172">
+        <f t="shared" si="8"/>
+        <v>65.760000000000005</v>
+      </c>
+      <c r="AO172">
+        <f t="shared" si="7"/>
+        <v>1.0036496350364963</v>
+      </c>
     </row>
-    <row r="173" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>172</v>
       </c>
@@ -20690,8 +22776,20 @@
       <c r="AL173">
         <v>1</v>
       </c>
+      <c r="AM173">
+        <f t="shared" si="6"/>
+        <v>50</v>
+      </c>
+      <c r="AN173">
+        <f t="shared" si="8"/>
+        <v>390.76</v>
+      </c>
+      <c r="AO173">
+        <f t="shared" si="7"/>
+        <v>0.12795577848295631</v>
+      </c>
     </row>
-    <row r="174" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>173</v>
       </c>
@@ -20797,8 +22895,20 @@
       <c r="AL174">
         <v>1</v>
       </c>
+      <c r="AM174">
+        <f t="shared" si="6"/>
+        <v>180</v>
+      </c>
+      <c r="AN174">
+        <f t="shared" si="8"/>
+        <v>180.76</v>
+      </c>
+      <c r="AO174">
+        <f t="shared" si="7"/>
+        <v>0.99579552998450993</v>
+      </c>
     </row>
-    <row r="175" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>174</v>
       </c>
@@ -20904,8 +23014,20 @@
       <c r="AL175">
         <v>1</v>
       </c>
+      <c r="AM175">
+        <f t="shared" si="6"/>
+        <v>201</v>
+      </c>
+      <c r="AN175">
+        <f t="shared" si="8"/>
+        <v>290.76</v>
+      </c>
+      <c r="AO175">
+        <f t="shared" si="7"/>
+        <v>0.69129178704085847</v>
+      </c>
     </row>
-    <row r="176" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>175</v>
       </c>
@@ -21011,8 +23133,20 @@
       <c r="AL176">
         <v>1</v>
       </c>
+      <c r="AM176">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AN176">
+        <f t="shared" si="8"/>
+        <v>290.76</v>
+      </c>
+      <c r="AO176">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="177" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>176</v>
       </c>
@@ -21118,8 +23252,20 @@
       <c r="AL177">
         <v>1</v>
       </c>
+      <c r="AM177">
+        <f t="shared" si="6"/>
+        <v>100</v>
+      </c>
+      <c r="AN177">
+        <f t="shared" si="8"/>
+        <v>440.76</v>
+      </c>
+      <c r="AO177">
+        <f t="shared" si="7"/>
+        <v>0.22688084218168619</v>
+      </c>
     </row>
-    <row r="178" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>177</v>
       </c>
@@ -21225,8 +23371,20 @@
       <c r="AL178">
         <v>1</v>
       </c>
+      <c r="AM178">
+        <f t="shared" si="6"/>
+        <v>400</v>
+      </c>
+      <c r="AN178">
+        <f t="shared" si="8"/>
+        <v>90.76</v>
+      </c>
+      <c r="AO178">
+        <f t="shared" si="7"/>
+        <v>4.4072278536800349</v>
+      </c>
     </row>
-    <row r="179" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>178</v>
       </c>
@@ -21332,8 +23490,20 @@
       <c r="AL179">
         <v>1</v>
       </c>
+      <c r="AM179">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="AN179">
+        <f t="shared" si="8"/>
+        <v>95.76</v>
+      </c>
+      <c r="AO179">
+        <f t="shared" si="7"/>
+        <v>5.2213868003341685E-2</v>
+      </c>
     </row>
-    <row r="180" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>179</v>
       </c>
@@ -21439,8 +23609,20 @@
       <c r="AL180">
         <v>1</v>
       </c>
+      <c r="AM180">
+        <f t="shared" si="6"/>
+        <v>50</v>
+      </c>
+      <c r="AN180">
+        <f t="shared" si="8"/>
+        <v>440.76</v>
+      </c>
+      <c r="AO180">
+        <f t="shared" si="7"/>
+        <v>0.1134404210908431</v>
+      </c>
     </row>
-    <row r="181" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>180</v>
       </c>
@@ -21546,8 +23728,20 @@
       <c r="AL181">
         <v>1</v>
       </c>
+      <c r="AM181">
+        <f t="shared" si="6"/>
+        <v>50</v>
+      </c>
+      <c r="AN181">
+        <f t="shared" si="8"/>
+        <v>490.76</v>
+      </c>
+      <c r="AO181">
+        <f t="shared" si="7"/>
+        <v>0.10188279403374359</v>
+      </c>
     </row>
-    <row r="182" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>181</v>
       </c>
@@ -21662,8 +23856,20 @@
       <c r="AL182">
         <v>1</v>
       </c>
+      <c r="AM182">
+        <f t="shared" si="6"/>
+        <v>436</v>
+      </c>
+      <c r="AN182">
+        <f t="shared" si="8"/>
+        <v>446.76</v>
+      </c>
+      <c r="AO182">
+        <f t="shared" si="7"/>
+        <v>0.97591548034739006</v>
+      </c>
     </row>
-    <row r="183" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>182</v>
       </c>
@@ -21769,8 +23975,20 @@
       <c r="AL183">
         <v>1</v>
       </c>
+      <c r="AM183">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AN183">
+        <f t="shared" si="8"/>
+        <v>5.76</v>
+      </c>
+      <c r="AO183">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="184" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>183</v>
       </c>
@@ -21876,8 +24094,20 @@
       <c r="AL184">
         <v>1</v>
       </c>
+      <c r="AM184">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AN184">
+        <f t="shared" si="8"/>
+        <v>40.76</v>
+      </c>
+      <c r="AO184">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="185" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>184</v>
       </c>
@@ -21983,8 +24213,20 @@
       <c r="AL185">
         <v>1</v>
       </c>
+      <c r="AM185">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AN185">
+        <f t="shared" si="8"/>
+        <v>10.76</v>
+      </c>
+      <c r="AO185">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="186" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>185</v>
       </c>
@@ -22090,8 +24332,20 @@
       <c r="AL186">
         <v>1</v>
       </c>
+      <c r="AM186">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AN186">
+        <f t="shared" si="8"/>
+        <v>10.76</v>
+      </c>
+      <c r="AO186">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="187" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>186</v>
       </c>
@@ -22197,8 +24451,20 @@
       <c r="AL187">
         <v>1</v>
       </c>
+      <c r="AM187">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="AN187">
+        <f t="shared" si="8"/>
+        <v>8.76</v>
+      </c>
+      <c r="AO187">
+        <f t="shared" si="7"/>
+        <v>0.34246575342465752</v>
+      </c>
     </row>
-    <row r="188" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>187</v>
       </c>
@@ -22304,8 +24570,20 @@
       <c r="AL188">
         <v>2</v>
       </c>
+      <c r="AM188">
+        <f t="shared" si="6"/>
+        <v>1.5</v>
+      </c>
+      <c r="AN188">
+        <f t="shared" si="8"/>
+        <v>5.74</v>
+      </c>
+      <c r="AO188">
+        <f t="shared" si="7"/>
+        <v>0.26132404181184671</v>
+      </c>
     </row>
-    <row r="189" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>188</v>
       </c>
@@ -22411,8 +24689,20 @@
       <c r="AL189">
         <v>2</v>
       </c>
+      <c r="AM189">
+        <f t="shared" si="6"/>
+        <v>4.9999999999999822E-2</v>
+      </c>
+      <c r="AN189">
+        <f t="shared" si="8"/>
+        <v>5.79</v>
+      </c>
+      <c r="AO189">
+        <f t="shared" si="7"/>
+        <v>8.6355785837650811E-3</v>
+      </c>
     </row>
-    <row r="190" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>189</v>
       </c>
@@ -22518,8 +24808,20 @@
       <c r="AL190">
         <v>1</v>
       </c>
+      <c r="AM190">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AN190">
+        <f t="shared" si="8"/>
+        <v>40.76</v>
+      </c>
+      <c r="AO190">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="191" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>190</v>
       </c>
@@ -22625,8 +24927,20 @@
       <c r="AL191">
         <v>1</v>
       </c>
+      <c r="AM191">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AN191">
+        <f t="shared" si="8"/>
+        <v>5.76</v>
+      </c>
+      <c r="AO191">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="192" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>191</v>
       </c>
@@ -22741,8 +25055,20 @@
       <c r="AL192">
         <v>1</v>
       </c>
+      <c r="AM192">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AN192">
+        <f t="shared" si="8"/>
+        <v>490.76</v>
+      </c>
+      <c r="AO192">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="193" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>192</v>
       </c>
@@ -22848,8 +25174,20 @@
       <c r="AL193">
         <v>1</v>
       </c>
+      <c r="AM193">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AN193">
+        <f t="shared" si="8"/>
+        <v>5.76</v>
+      </c>
+      <c r="AO193">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="194" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>193</v>
       </c>
@@ -22964,8 +25302,20 @@
       <c r="AL194">
         <v>2</v>
       </c>
+      <c r="AM194">
+        <f t="shared" si="6"/>
+        <v>85</v>
+      </c>
+      <c r="AN194">
+        <f t="shared" si="8"/>
+        <v>90.76</v>
+      </c>
+      <c r="AO194">
+        <f t="shared" si="7"/>
+        <v>0.93653591890700749</v>
+      </c>
     </row>
-    <row r="195" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>194</v>
       </c>
@@ -23071,8 +25421,20 @@
       <c r="AL195">
         <v>1</v>
       </c>
+      <c r="AM195">
+        <f t="shared" ref="AM195:AM197" si="9">ABS(SUM(AE195-C195))</f>
+        <v>0</v>
+      </c>
+      <c r="AN195">
+        <f t="shared" si="8"/>
+        <v>490.76</v>
+      </c>
+      <c r="AO195">
+        <f t="shared" ref="AO195:AO197" si="10">SUM(AM195/AN195)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="196" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>195</v>
       </c>
@@ -23178,8 +25540,20 @@
       <c r="AL196">
         <v>2</v>
       </c>
+      <c r="AM196">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="AN196">
+        <f t="shared" si="8"/>
+        <v>10.76</v>
+      </c>
+      <c r="AO196">
+        <f t="shared" si="10"/>
+        <v>0.92936802973977695</v>
+      </c>
     </row>
-    <row r="197" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>196</v>
       </c>
@@ -23284,6 +25658,18 @@
       </c>
       <c r="AL197">
         <v>1</v>
+      </c>
+      <c r="AM197">
+        <f t="shared" si="9"/>
+        <v>200</v>
+      </c>
+      <c r="AN197">
+        <f t="shared" si="8"/>
+        <v>345.76</v>
+      </c>
+      <c r="AO197">
+        <f t="shared" si="10"/>
+        <v>0.57843590930124944</v>
       </c>
     </row>
   </sheetData>

</xml_diff>